<commit_message>
modified to work on cloud shell
</commit_message>
<xml_diff>
--- a/evaluation_files/EMO, POLICY & VAS QA_updated.xlsx
+++ b/evaluation_files/EMO, POLICY & VAS QA_updated.xlsx
@@ -5,20 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhammad.s.safian\OneDrive - Avanade\Project\MAIN_PROJECT\_avanade_main\_avanade_main\_01_prudential\PRUHK-AgenticRAG-V4\evaluation_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://avanade-my.sharepoint.com/personal/aina_rahim_avanade_com/Documents/Microsoft Teams Chat Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147EC42E-6D72-4B05-BEFF-67AFB9D816F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7461B37-1A06-431D-B135-E67A05D2325C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29055" yWindow="16125" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$244</definedName>
-  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1323" uniqueCount="648">
   <si>
     <t>Folder</t>
   </si>
@@ -3454,12 +3451,54 @@
     <t>The Treatment Sure offers Global Expert Medical Opinion and Medical Concierge services… If the insured person chooses to receive treatment abroad, they will be responsible for all fees and charges required for travel and accommodation and related items
 The amount you can claim for treatment expenses is subject to the benefit limit of your plan… You will need to get our pre-authorisation before your treatment.</t>
   </si>
+  <si>
+    <t>Does Encash Hospital Cash Savings Insurance provide death benefit?</t>
+  </si>
+  <si>
+    <t>Yes, it pays a death benefit equal to current sum assured and terminal bonus</t>
+  </si>
+  <si>
+    <t>We will pay 100% of the current sum assured and terminal bonus as the Death Benefit</t>
+  </si>
+  <si>
+    <t>Can I reduce my deductible under PremierFlex Medical Plan?</t>
+  </si>
+  <si>
+    <t>You can gear up your protection by reducing your deductible once in your lifetime</t>
+  </si>
+  <si>
+    <t>Yes, you can reduce it once in your lifetime at specified ages</t>
+  </si>
+  <si>
+    <t>Can I use Medical Green Channel outside Mainland China?</t>
+  </si>
+  <si>
+    <t>No, it applies only to selected hospitals in Mainland China</t>
+  </si>
+  <si>
+    <t>Selected hospitals in Mainland China</t>
+  </si>
+  <si>
+    <t>For PruHealth VHIS VIP Plan, are value-added services guaranteed for life?</t>
+  </si>
+  <si>
+    <t>No, they are subject to terms and conditions</t>
+  </si>
+  <si>
+    <t>Does PRUmyhealth prestige medical plan include outpatient benefits?</t>
+  </si>
+  <si>
+    <t>Outpatient benefits are available through a designated supplementary benefit</t>
+  </si>
+  <si>
+    <t>You can top up your plan with our tailored outpatient benefit</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3478,6 +3517,19 @@
       <color rgb="FFFAFAFA"/>
       <name val="Source Sans Pro"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -3551,7 +3603,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -3586,14 +3638,13 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3611,6 +3662,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3898,23 +3953,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:E244"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B9:B10"/>
+    <sheetView zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" customWidth="1"/>
-    <col min="2" max="2" width="53.5546875" customWidth="1"/>
-    <col min="3" max="3" width="34.5546875" customWidth="1"/>
-    <col min="4" max="4" width="54.44140625" customWidth="1"/>
-    <col min="5" max="5" width="201.77734375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="19.54296875" customWidth="1"/>
+    <col min="2" max="2" width="53.54296875" customWidth="1"/>
+    <col min="3" max="3" width="34.54296875" customWidth="1"/>
+    <col min="4" max="4" width="54.453125" customWidth="1"/>
+    <col min="5" max="5" width="201.81640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3931,7 +3985,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -3948,7 +4002,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -3965,7 +4019,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="135" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -3982,7 +4036,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -3999,7 +4053,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -4016,7 +4070,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -4033,7 +4087,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -4050,7 +4104,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
@@ -4067,7 +4121,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
@@ -4084,7 +4138,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
@@ -4101,7 +4155,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -4118,7 +4172,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
@@ -4135,7 +4189,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
@@ -4152,7 +4206,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>5</v>
       </c>
@@ -4169,7 +4223,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>5</v>
       </c>
@@ -4186,7 +4240,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -4203,7 +4257,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
@@ -4220,7 +4274,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>48</v>
       </c>
@@ -4237,7 +4291,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>48</v>
       </c>
@@ -4254,7 +4308,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>48</v>
       </c>
@@ -4271,7 +4325,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>48</v>
       </c>
@@ -4288,7 +4342,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>48</v>
       </c>
@@ -4305,7 +4359,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>48</v>
       </c>
@@ -4322,7 +4376,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>48</v>
       </c>
@@ -4339,7 +4393,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="172.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
         <v>48</v>
       </c>
@@ -4356,7 +4410,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
         <v>48</v>
       </c>
@@ -4373,7 +4427,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
         <v>48</v>
       </c>
@@ -4390,7 +4444,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
         <v>48</v>
       </c>
@@ -4407,7 +4461,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A30" s="6" t="s">
         <v>48</v>
       </c>
@@ -4424,7 +4478,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
         <v>48</v>
       </c>
@@ -4441,7 +4495,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
         <v>48</v>
       </c>
@@ -4458,7 +4512,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
         <v>48</v>
       </c>
@@ -4475,7 +4529,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
         <v>48</v>
       </c>
@@ -4492,7 +4546,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
         <v>48</v>
       </c>
@@ -4509,7 +4563,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
         <v>48</v>
       </c>
@@ -4526,7 +4580,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
         <v>48</v>
       </c>
@@ -4543,7 +4597,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A38" s="6" t="s">
         <v>48</v>
       </c>
@@ -4560,7 +4614,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A39" s="6" t="s">
         <v>48</v>
       </c>
@@ -4577,7 +4631,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="6" t="s">
         <v>48</v>
       </c>
@@ -4594,7 +4648,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A41" s="6" t="s">
         <v>48</v>
       </c>
@@ -4611,7 +4665,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A42" s="6" t="s">
         <v>48</v>
       </c>
@@ -4628,7 +4682,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="144" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A43" s="8" t="s">
         <v>48</v>
       </c>
@@ -4645,7 +4699,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="144" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A44" s="8" t="s">
         <v>48</v>
       </c>
@@ -4662,7 +4716,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A45" s="8" t="s">
         <v>48</v>
       </c>
@@ -4679,7 +4733,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A46" s="8" t="s">
         <v>48</v>
       </c>
@@ -4696,7 +4750,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A47" s="8" t="s">
         <v>48</v>
       </c>
@@ -4713,7 +4767,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A48" s="8" t="s">
         <v>48</v>
       </c>
@@ -4730,7 +4784,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A49" s="8" t="s">
         <v>48</v>
       </c>
@@ -4747,7 +4801,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A50" s="8" t="s">
         <v>48</v>
       </c>
@@ -4764,7 +4818,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A51" s="8" t="s">
         <v>48</v>
       </c>
@@ -4781,7 +4835,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="8" t="s">
         <v>48</v>
       </c>
@@ -4798,7 +4852,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A53" s="8" t="s">
         <v>48</v>
       </c>
@@ -4815,7 +4869,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="8" t="s">
         <v>48</v>
       </c>
@@ -4832,7 +4886,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A55" s="8" t="s">
         <v>48</v>
       </c>
@@ -4849,7 +4903,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="144" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A56" s="8" t="s">
         <v>48</v>
       </c>
@@ -4866,7 +4920,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="144" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A57" s="8" t="s">
         <v>48</v>
       </c>
@@ -4883,7 +4937,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A58" s="8" t="s">
         <v>48</v>
       </c>
@@ -4900,7 +4954,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="144" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A59" s="8" t="s">
         <v>48</v>
       </c>
@@ -4917,7 +4971,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A60" s="8" t="s">
         <v>48</v>
       </c>
@@ -4934,7 +4988,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A61" s="8" t="s">
         <v>48</v>
       </c>
@@ -4951,7 +5005,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="8" t="s">
         <v>48</v>
       </c>
@@ -4968,7 +5022,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="8" t="s">
         <v>48</v>
       </c>
@@ -4985,7 +5039,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="8" t="s">
         <v>48</v>
       </c>
@@ -5002,7 +5056,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="8" t="s">
         <v>48</v>
       </c>
@@ -5019,7 +5073,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="8" t="s">
         <v>48</v>
       </c>
@@ -5036,7 +5090,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="8" t="s">
         <v>48</v>
       </c>
@@ -5053,7 +5107,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="8" t="s">
         <v>48</v>
       </c>
@@ -5070,7 +5124,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="8" t="s">
         <v>48</v>
       </c>
@@ -5087,7 +5141,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A70" s="8" t="s">
         <v>48</v>
       </c>
@@ -5104,7 +5158,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A71" s="6" t="s">
         <v>180</v>
       </c>
@@ -5121,7 +5175,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A72" s="6" t="s">
         <v>180</v>
       </c>
@@ -5138,7 +5192,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A73" s="6" t="s">
         <v>180</v>
       </c>
@@ -5155,7 +5209,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A74" s="6" t="s">
         <v>180</v>
       </c>
@@ -5172,7 +5226,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="6" t="s">
         <v>180</v>
       </c>
@@ -5189,7 +5243,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A76" s="6" t="s">
         <v>180</v>
       </c>
@@ -5206,7 +5260,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A77" s="6" t="s">
         <v>180</v>
       </c>
@@ -5223,7 +5277,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A78" s="6" t="s">
         <v>180</v>
       </c>
@@ -5240,7 +5294,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A79" s="6" t="s">
         <v>180</v>
       </c>
@@ -5257,7 +5311,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="6" t="s">
         <v>180</v>
       </c>
@@ -5274,7 +5328,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A81" s="6" t="s">
         <v>180</v>
       </c>
@@ -5291,7 +5345,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A82" s="6" t="s">
         <v>180</v>
       </c>
@@ -5308,7 +5362,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="201.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="s">
         <v>180</v>
       </c>
@@ -5325,7 +5379,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="201.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="s">
         <v>180</v>
       </c>
@@ -5342,7 +5396,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A85" s="4" t="s">
         <v>180</v>
       </c>
@@ -5359,7 +5413,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="s">
         <v>180</v>
       </c>
@@ -5376,7 +5430,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A87" s="4" t="s">
         <v>180</v>
       </c>
@@ -5393,7 +5447,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="201.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="s">
         <v>180</v>
       </c>
@@ -5410,7 +5464,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="216" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A89" s="4" t="s">
         <v>180</v>
       </c>
@@ -5427,7 +5481,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="216" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A90" s="4" t="s">
         <v>180</v>
       </c>
@@ -5444,7 +5498,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A91" s="4" t="s">
         <v>180</v>
       </c>
@@ -5461,7 +5515,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A92" s="4" t="s">
         <v>180</v>
       </c>
@@ -5478,7 +5532,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A93" s="10" t="s">
         <v>180</v>
       </c>
@@ -5495,7 +5549,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="10" t="s">
         <v>180</v>
       </c>
@@ -5512,7 +5566,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A95" s="10" t="s">
         <v>180</v>
       </c>
@@ -5529,7 +5583,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="10" t="s">
         <v>180</v>
       </c>
@@ -5546,7 +5600,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="10" t="s">
         <v>180</v>
       </c>
@@ -5563,7 +5617,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="10" t="s">
         <v>180</v>
       </c>
@@ -5580,7 +5634,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A99" s="10" t="s">
         <v>180</v>
       </c>
@@ -5597,7 +5651,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A100" s="10" t="s">
         <v>180</v>
       </c>
@@ -5614,7 +5668,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="10" t="s">
         <v>180</v>
       </c>
@@ -5631,7 +5685,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A102" s="10" t="s">
         <v>180</v>
       </c>
@@ -5648,7 +5702,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A103" s="8" t="s">
         <v>180</v>
       </c>
@@ -5665,7 +5719,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="8" t="s">
         <v>180</v>
       </c>
@@ -5682,7 +5736,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="8" t="s">
         <v>180</v>
       </c>
@@ -5699,7 +5753,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A106" s="8" t="s">
         <v>180</v>
       </c>
@@ -5716,7 +5770,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="8" t="s">
         <v>180</v>
       </c>
@@ -5733,7 +5787,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="8" t="s">
         <v>180</v>
       </c>
@@ -5750,7 +5804,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="109" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="8" t="s">
         <v>180</v>
       </c>
@@ -5767,7 +5821,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A110" s="8" t="s">
         <v>180</v>
       </c>
@@ -5784,7 +5838,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A111" s="8" t="s">
         <v>180</v>
       </c>
@@ -5801,7 +5855,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A112" s="8" t="s">
         <v>180</v>
       </c>
@@ -5818,7 +5872,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="144" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A113" s="6" t="s">
         <v>180</v>
       </c>
@@ -5835,7 +5889,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="144" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A114" s="6" t="s">
         <v>180</v>
       </c>
@@ -5852,7 +5906,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="144" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A115" s="6" t="s">
         <v>180</v>
       </c>
@@ -5869,7 +5923,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A116" s="6" t="s">
         <v>180</v>
       </c>
@@ -5886,7 +5940,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A117" s="6" t="s">
         <v>180</v>
       </c>
@@ -5903,7 +5957,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A118" s="6" t="s">
         <v>180</v>
       </c>
@@ -5920,7 +5974,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A119" s="6" t="s">
         <v>180</v>
       </c>
@@ -5937,7 +5991,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A120" s="6" t="s">
         <v>180</v>
       </c>
@@ -5954,7 +6008,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="6" t="s">
         <v>180</v>
       </c>
@@ -5971,7 +6025,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="6" t="s">
         <v>180</v>
       </c>
@@ -5988,7 +6042,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A123" s="12" t="s">
         <v>180</v>
       </c>
@@ -6005,7 +6059,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="12" t="s">
         <v>180</v>
       </c>
@@ -6022,7 +6076,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A125" s="12" t="s">
         <v>180</v>
       </c>
@@ -6039,7 +6093,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A126" s="12" t="s">
         <v>180</v>
       </c>
@@ -6056,7 +6110,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A127" s="12" t="s">
         <v>180</v>
       </c>
@@ -6073,7 +6127,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="12" t="s">
         <v>180</v>
       </c>
@@ -6090,7 +6144,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="12" t="s">
         <v>180</v>
       </c>
@@ -6107,7 +6161,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A130" s="12" t="s">
         <v>180</v>
       </c>
@@ -6124,7 +6178,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A131" s="12" t="s">
         <v>180</v>
       </c>
@@ -6141,7 +6195,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A132" s="12" t="s">
         <v>180</v>
       </c>
@@ -6158,7 +6212,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A133" s="4" t="s">
         <v>180</v>
       </c>
@@ -6175,7 +6229,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A134" s="4" t="s">
         <v>180</v>
       </c>
@@ -6192,7 +6246,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="4" t="s">
         <v>180</v>
       </c>
@@ -6209,7 +6263,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A136" s="4" t="s">
         <v>180</v>
       </c>
@@ -6226,7 +6280,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A137" s="4" t="s">
         <v>180</v>
       </c>
@@ -6243,7 +6297,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A138" s="4" t="s">
         <v>180</v>
       </c>
@@ -6260,7 +6314,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A139" s="4" t="s">
         <v>180</v>
       </c>
@@ -6277,7 +6331,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A140" s="4" t="s">
         <v>180</v>
       </c>
@@ -6294,7 +6348,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A141" s="4" t="s">
         <v>180</v>
       </c>
@@ -6311,7 +6365,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A142" s="4" t="s">
         <v>180</v>
       </c>
@@ -6328,7 +6382,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A143" s="8" t="s">
         <v>362</v>
       </c>
@@ -6345,7 +6399,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A144" s="8" t="s">
         <v>362</v>
       </c>
@@ -6362,7 +6416,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="374.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" ht="377" x14ac:dyDescent="0.35">
       <c r="A145" s="8" t="s">
         <v>362</v>
       </c>
@@ -6379,7 +6433,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A146" s="8" t="s">
         <v>362</v>
       </c>
@@ -6396,7 +6450,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A147" s="8" t="s">
         <v>362</v>
       </c>
@@ -6413,7 +6467,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="374.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" ht="377" x14ac:dyDescent="0.35">
       <c r="A148" s="8" t="s">
         <v>362</v>
       </c>
@@ -6430,7 +6484,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="149" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="8" t="s">
         <v>362</v>
       </c>
@@ -6447,7 +6501,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="150" spans="1:5" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A150" s="8" t="s">
         <v>362</v>
       </c>
@@ -6464,7 +6518,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="151" spans="1:5" ht="374.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" ht="377" x14ac:dyDescent="0.35">
       <c r="A151" s="8" t="s">
         <v>362</v>
       </c>
@@ -6481,7 +6535,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="152" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A152" s="8" t="s">
         <v>362</v>
       </c>
@@ -6498,7 +6552,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="153" spans="1:5" ht="374.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" ht="377" x14ac:dyDescent="0.35">
       <c r="A153" s="8" t="s">
         <v>362</v>
       </c>
@@ -6515,7 +6569,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="374.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" ht="377" x14ac:dyDescent="0.35">
       <c r="A154" s="8" t="s">
         <v>362</v>
       </c>
@@ -6532,7 +6586,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="374.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" ht="377" x14ac:dyDescent="0.35">
       <c r="A155" s="8" t="s">
         <v>362</v>
       </c>
@@ -6549,7 +6603,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A156" s="8" t="s">
         <v>362</v>
       </c>
@@ -6566,7 +6620,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="157" spans="1:5" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A157" s="8" t="s">
         <v>362</v>
       </c>
@@ -6583,7 +6637,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="158" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A158" s="8" t="s">
         <v>362</v>
       </c>
@@ -6600,7 +6654,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="144" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A159" s="14" t="s">
         <v>362</v>
       </c>
@@ -6617,7 +6671,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="160" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A160" s="14" t="s">
         <v>362</v>
       </c>
@@ -6634,7 +6688,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="161" spans="1:5" ht="144" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A161" s="14" t="s">
         <v>362</v>
       </c>
@@ -6651,7 +6705,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="162" spans="1:5" ht="144" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A162" s="14" t="s">
         <v>362</v>
       </c>
@@ -6668,7 +6722,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="163" spans="1:5" ht="144" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A163" s="14" t="s">
         <v>362</v>
       </c>
@@ -6685,7 +6739,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="164" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A164" s="14" t="s">
         <v>362</v>
       </c>
@@ -6702,7 +6756,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A165" s="14" t="s">
         <v>362</v>
       </c>
@@ -6719,7 +6773,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="166" spans="1:5" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A166" s="14" t="s">
         <v>362</v>
       </c>
@@ -6736,7 +6790,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="167" spans="1:5" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A167" s="14" t="s">
         <v>362</v>
       </c>
@@ -6753,7 +6807,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="168" spans="1:5" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A168" s="10" t="s">
         <v>362</v>
       </c>
@@ -6770,7 +6824,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="169" spans="1:5" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A169" s="10" t="s">
         <v>362</v>
       </c>
@@ -6787,7 +6841,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="170" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A170" s="10" t="s">
         <v>362</v>
       </c>
@@ -6804,7 +6858,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="171" spans="1:5" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A171" s="10" t="s">
         <v>362</v>
       </c>
@@ -6821,7 +6875,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="172" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A172" s="10" t="s">
         <v>362</v>
       </c>
@@ -6838,7 +6892,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="173" spans="1:5" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A173" s="10" t="s">
         <v>362</v>
       </c>
@@ -6855,7 +6909,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="174" spans="1:5" ht="259.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A174" s="10" t="s">
         <v>362</v>
       </c>
@@ -6872,7 +6926,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="175" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A175" s="10" t="s">
         <v>362</v>
       </c>
@@ -6889,7 +6943,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="176" spans="1:5" ht="187.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A176" s="10" t="s">
         <v>362</v>
       </c>
@@ -6906,7 +6960,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="177" spans="1:5" ht="187.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A177" s="6" t="s">
         <v>362</v>
       </c>
@@ -6923,7 +6977,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="178" spans="1:5" ht="187.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A178" s="6" t="s">
         <v>362</v>
       </c>
@@ -6940,7 +6994,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="179" spans="1:5" ht="187.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A179" s="6" t="s">
         <v>362</v>
       </c>
@@ -6957,7 +7011,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="180" spans="1:5" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A180" s="6" t="s">
         <v>362</v>
       </c>
@@ -6974,7 +7028,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="181" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A181" s="6" t="s">
         <v>362</v>
       </c>
@@ -6991,7 +7045,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="182" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A182" s="6" t="s">
         <v>362</v>
       </c>
@@ -7008,7 +7062,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="183" spans="1:5" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A183" s="6" t="s">
         <v>362</v>
       </c>
@@ -7025,7 +7079,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="184" spans="1:5" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A184" s="8" t="s">
         <v>362</v>
       </c>
@@ -7042,7 +7096,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="185" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A185" s="8" t="s">
         <v>362</v>
       </c>
@@ -7059,7 +7113,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="186" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A186" s="8" t="s">
         <v>362</v>
       </c>
@@ -7076,7 +7130,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="187" spans="1:5" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A187" s="8" t="s">
         <v>362</v>
       </c>
@@ -7093,7 +7147,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="188" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A188" s="8" t="s">
         <v>362</v>
       </c>
@@ -7110,7 +7164,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="189" spans="1:5" ht="144" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A189" s="8" t="s">
         <v>362</v>
       </c>
@@ -7127,7 +7181,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="190" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A190" s="8" t="s">
         <v>362</v>
       </c>
@@ -7144,7 +7198,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="191" spans="1:5" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A191" s="4" t="s">
         <v>362</v>
       </c>
@@ -7161,7 +7215,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="192" spans="1:5" ht="216" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A192" s="4" t="s">
         <v>362</v>
       </c>
@@ -7178,7 +7232,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="193" spans="1:5" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A193" s="4" t="s">
         <v>362</v>
       </c>
@@ -7195,7 +7249,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="194" spans="1:5" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A194" s="4" t="s">
         <v>362</v>
       </c>
@@ -7212,7 +7266,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="195" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A195" s="4" t="s">
         <v>362</v>
       </c>
@@ -7229,7 +7283,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="196" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A196" s="4" t="s">
         <v>362</v>
       </c>
@@ -7246,7 +7300,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="197" spans="1:5" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A197" s="4" t="s">
         <v>362</v>
       </c>
@@ -7263,7 +7317,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="198" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A198" s="4" t="s">
         <v>362</v>
       </c>
@@ -7280,7 +7334,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="199" spans="1:5" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A199" s="4" t="s">
         <v>362</v>
       </c>
@@ -7297,7 +7351,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="200" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A200" s="6" t="s">
         <v>362</v>
       </c>
@@ -7314,7 +7368,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="201" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A201" s="6" t="s">
         <v>362</v>
       </c>
@@ -7331,7 +7385,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="202" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A202" s="6" t="s">
         <v>362</v>
       </c>
@@ -7348,7 +7402,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="203" spans="1:5" ht="144" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A203" s="6" t="s">
         <v>362</v>
       </c>
@@ -7365,7 +7419,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="204" spans="1:5" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A204" s="6" t="s">
         <v>362</v>
       </c>
@@ -7382,7 +7436,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="205" spans="1:5" ht="144" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A205" s="6" t="s">
         <v>362</v>
       </c>
@@ -7399,7 +7453,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="206" spans="1:5" ht="144" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A206" s="6" t="s">
         <v>362</v>
       </c>
@@ -7416,7 +7470,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="207" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A207" s="10" t="s">
         <v>362</v>
       </c>
@@ -7433,7 +7487,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="208" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A208" s="10" t="s">
         <v>362</v>
       </c>
@@ -7450,7 +7504,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="209" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A209" s="10" t="s">
         <v>362</v>
       </c>
@@ -7467,7 +7521,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="210" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A210" s="8" t="s">
         <v>362</v>
       </c>
@@ -7484,7 +7538,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="211" spans="1:5" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A211" s="8" t="s">
         <v>362</v>
       </c>
@@ -7501,7 +7555,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="212" spans="1:5" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A212" s="8" t="s">
         <v>362</v>
       </c>
@@ -7518,7 +7572,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="213" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A213" s="8" t="s">
         <v>362</v>
       </c>
@@ -7535,7 +7589,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="214" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A214" s="8" t="s">
         <v>362</v>
       </c>
@@ -7552,7 +7606,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="215" spans="1:5" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A215" s="8" t="s">
         <v>362</v>
       </c>
@@ -7569,7 +7623,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="216" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A216" s="8" t="s">
         <v>362</v>
       </c>
@@ -7586,7 +7640,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="217" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A217" s="8" t="s">
         <v>362</v>
       </c>
@@ -7603,7 +7657,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="218" spans="1:5" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A218" s="4" t="s">
         <v>362</v>
       </c>
@@ -7620,7 +7674,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="219" spans="1:5" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A219" s="4" t="s">
         <v>362</v>
       </c>
@@ -7637,7 +7691,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="220" spans="1:5" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A220" s="4" t="s">
         <v>362</v>
       </c>
@@ -7654,7 +7708,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="221" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A221" s="4" t="s">
         <v>362</v>
       </c>
@@ -7671,7 +7725,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="222" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A222" s="4" t="s">
         <v>362</v>
       </c>
@@ -7688,7 +7742,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="223" spans="1:5" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A223" s="4" t="s">
         <v>362</v>
       </c>
@@ -7705,7 +7759,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="224" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A224" s="4" t="s">
         <v>362</v>
       </c>
@@ -7722,7 +7776,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="225" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A225" s="4" t="s">
         <v>362</v>
       </c>
@@ -7739,7 +7793,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="226" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A226" s="8" t="s">
         <v>362</v>
       </c>
@@ -7756,7 +7810,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="227" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A227" s="8" t="s">
         <v>362</v>
       </c>
@@ -7773,7 +7827,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="228" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A228" s="8" t="s">
         <v>362</v>
       </c>
@@ -7790,7 +7844,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="229" spans="1:5" ht="259.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A229" s="8" t="s">
         <v>362</v>
       </c>
@@ -7807,7 +7861,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="230" spans="1:5" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A230" s="8" t="s">
         <v>362</v>
       </c>
@@ -7824,7 +7878,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="231" spans="1:5" ht="259.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A231" s="8" t="s">
         <v>362</v>
       </c>
@@ -7841,7 +7895,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="232" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A232" s="8" t="s">
         <v>362</v>
       </c>
@@ -7858,7 +7912,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="233" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A233" s="10" t="s">
         <v>362</v>
       </c>
@@ -7875,7 +7929,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="234" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A234" s="10" t="s">
         <v>362</v>
       </c>
@@ -7892,7 +7946,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="235" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A235" s="10" t="s">
         <v>362</v>
       </c>
@@ -7909,7 +7963,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="236" spans="1:5" ht="259.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A236" s="10" t="s">
         <v>362</v>
       </c>
@@ -7926,7 +7980,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="237" spans="1:5" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A237" s="10" t="s">
         <v>362</v>
       </c>
@@ -7943,7 +7997,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="238" spans="1:5" ht="259.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A238" s="10" t="s">
         <v>362</v>
       </c>
@@ -7960,7 +8014,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="239" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A239" s="10" t="s">
         <v>362</v>
       </c>
@@ -7977,7 +8031,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="240" spans="1:5" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A240" s="6" t="s">
         <v>362</v>
       </c>
@@ -7994,7 +8048,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="241" spans="1:5" ht="144" hidden="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A241" s="6" t="s">
         <v>362</v>
       </c>
@@ -8011,7 +8065,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="242" spans="1:5" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A242" s="6" t="s">
         <v>362</v>
       </c>
@@ -8028,7 +8082,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="243" spans="1:5" ht="144" hidden="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A243" s="6" t="s">
         <v>362</v>
       </c>
@@ -8045,7 +8099,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="244" spans="1:5" ht="144" hidden="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A244" s="6" t="s">
         <v>362</v>
       </c>
@@ -8063,317 +8117,385 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E244" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="EMO"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D313330E-9F3A-40CB-814C-B0D03F27DB97}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="66" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.77734375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.77734375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="58.21875" customWidth="1"/>
-    <col min="6" max="6" width="79.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.7265625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="66" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.81640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="58.26953125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="79.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:7" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="B2" s="17" t="s">
+        <v>580</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>603</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>600</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="E2" s="17" t="s">
         <v>604</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="F2" s="17" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="B3" s="17" t="s">
+        <v>581</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>612</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>599</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>605</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="B4" s="17" t="s">
+        <v>582</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>602</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>601</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>609</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B5" s="17" t="s">
         <v>580</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>603</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
-        <v>599</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>605</v>
-      </c>
-      <c r="C3" s="17" t="s">
+      <c r="C5" s="17" t="s">
+        <v>584</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>402</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>586</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B6" s="17" t="s">
+        <v>580</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>584</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>585</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>587</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B7" s="17" t="s">
+        <v>580</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>584</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>590</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>591</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="B8" s="17" t="s">
         <v>581</v>
       </c>
-      <c r="D3" s="17" t="s">
-        <v>612</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
-        <v>601</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>609</v>
-      </c>
-      <c r="C4" s="17" t="s">
+      <c r="C8" s="17" t="s">
+        <v>584</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>593</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>594</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="B9" s="17" t="s">
+        <v>581</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>584</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>596</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="17" t="s">
         <v>582</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>602</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
-        <v>402</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>586</v>
-      </c>
-      <c r="C5" s="17" t="s">
+      <c r="C10" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>607</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>608</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="B11" s="17" t="s">
+        <v>582</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>584</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>615</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>632</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="348" x14ac:dyDescent="0.35">
+      <c r="B12" s="17" t="s">
+        <v>582</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>627</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>628</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="G12" s="16"/>
+    </row>
+    <row r="13" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="17" t="s">
+        <v>582</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>625</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>631</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>630</v>
+      </c>
+      <c r="G13" s="18"/>
+    </row>
+    <row r="14" spans="1:7" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="B14" s="17" t="s">
         <v>580</v>
       </c>
-      <c r="D5" s="17" t="s">
-        <v>584</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
-        <v>585</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>587</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>580</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>584</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>590</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>591</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>580</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>584</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
-        <v>593</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>594</v>
-      </c>
-      <c r="C8" s="17" t="s">
+      <c r="C14" s="17" t="s">
+        <v>618</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>617</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>614</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="261" x14ac:dyDescent="0.35">
+      <c r="B15" s="17" t="s">
         <v>581</v>
       </c>
-      <c r="D8" s="17" t="s">
-        <v>584</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>596</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>597</v>
-      </c>
-      <c r="C9" s="17" t="s">
+      <c r="C15" s="17" t="s">
+        <v>623</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>624</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>626</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="232" x14ac:dyDescent="0.35">
+      <c r="B16" s="17" t="s">
+        <v>582</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>619</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>620</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>621</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B17" s="19" t="s">
         <v>581</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>584</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
-        <v>607</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>608</v>
-      </c>
-      <c r="C10" s="17" t="s">
+      <c r="C17" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>635</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B18" s="17" t="s">
         <v>582</v>
       </c>
-      <c r="D10" s="17" t="s">
-        <v>213</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
-        <v>615</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>632</v>
-      </c>
-      <c r="C11" s="17" t="s">
+      <c r="C18" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B19" s="17" t="s">
         <v>582</v>
       </c>
-      <c r="D11" s="17" t="s">
-        <v>584</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="345.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
-        <v>627</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>628</v>
-      </c>
-      <c r="C12" s="17" t="s">
+      <c r="C19" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B20" s="17" t="s">
         <v>582</v>
       </c>
-      <c r="D12" s="17" t="s">
-        <v>266</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
-        <v>625</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>631</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>582</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>238</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>630</v>
-      </c>
-      <c r="F13" s="18"/>
-    </row>
-    <row r="14" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="17" t="s">
-        <v>617</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>614</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>580</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>618</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="216" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
-        <v>624</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>621</v>
-      </c>
-      <c r="C15" s="17" t="s">
+      <c r="C20" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B21" s="19" t="s">
         <v>581</v>
       </c>
-      <c r="D15" s="17" t="s">
-        <v>623</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="259.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
-        <v>620</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>626</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>582</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C17" s="16"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C18" s="16"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C19" s="16"/>
+      <c r="C21" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>647</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8382,6 +8504,6 @@
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{5fae8262-b78e-4366-8929-a5d6aac95320}" enabled="1" method="Standard" siteId="{cf36141c-ddd7-45a7-b073-111f66d0b30c}" contentBits="0" removed="0"/>
+  <clbl:label id="{5fae8262-b78e-4366-8929-a5d6aac95320}" enabled="1" method="Standard" siteId="{cf36141c-ddd7-45a7-b073-111f66d0b30c}" removed="0"/>
 </clbl:labelList>
 </file>
</xml_diff>

<commit_message>
update evaluation lifecycle for corpus filtering
</commit_message>
<xml_diff>
--- a/evaluation_files/EMO, POLICY & VAS QA_updated.xlsx
+++ b/evaluation_files/EMO, POLICY & VAS QA_updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\458840\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2388A05-791A-4F78-A108-3F5075F352E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCEBE56-AAC3-4F1E-A34C-574AB5D97310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="652">
   <si>
     <t>Folder</t>
   </si>
@@ -3149,25 +3149,6 @@
   </si>
   <si>
     <t>What's Treatment Sure?</t>
-  </si>
-  <si>
-    <t>Treatment Sure is a one-stop medical advisory service provided by Prudential in collaboration with its partner, Teladoc Health. This service includes:
-Global Second Medical Opinions: Offers independent medical opinions from an extensive network of over 50,000 global medical experts covering more than 450 specialties and sub-specialties. This helps you verify diagnoses and explore the most suitable treatments for your condition.
-Medical Concierge for Overseas Treatment: If you need treatment abroad, the service provides a dedicated physician case manager to guide you throughout your medical journey. This includes identifying suitable specialists around the world, arranging appointments, translation services, and even follow-ups post-treatment.
-Comprehensive Support: A dedicated physician case manager is assigned to support you at every step, answering your questions and ensuring personalized care.
-The service has benefited over 35 million customers across 130 countries, assuring peace of mind by helping in making informed health decisions.
-How Does It Work?
-Step 1: A physician case manager is assigned to you.
-Step 2: The manager gathers details about your medical condition.
-Step 3: Suitable global experts are identified and consulted.
-Step 4: You receive a personalized second medical opinion report in your language.
-Step 5: If you opt for overseas treatment, the manager organizes specialist options, appointments, and logistics.
-Step 6: Post-treatment, the manager follows up on your recovery.
-Contact Details
-For activation or queries:
-Hong Kong SAR: (852) 8229 2880
-Mainland China: (86) 400 920 6012
-Full details can be found in the [Treatment Sure document](gs://prudential-poc/vas/Treatment Sure.docx).</t>
   </si>
   <si>
     <t>Skip links
@@ -3360,9 +3341,6 @@
   </si>
   <si>
     <t>Policy specific QA</t>
-  </si>
-  <si>
-    <t>What's Treatment Sure? (Authenticated policy holder for PRUmyhealth prestige medical plan)</t>
   </si>
   <si>
     <t>The Treatment Sure service is a value-added feature associated with the PRUmyhealth Prestige Medical Plan designed to provide you with enhanced medical support services. Here's what it includes:
@@ -3608,13 +3586,7 @@
     <t>gs://guide-care-poc/policy/pruhealth-corechoice-medical-plan-product-brochure.pdf</t>
   </si>
   <si>
-    <t>What is the annual benefit limit under CoreChoice?</t>
-  </si>
-  <si>
     <t>The annual benefit limit is HKD 420,000</t>
-  </si>
-  <si>
-    <t>Who is eligible to apply for CoreChoice?</t>
   </si>
   <si>
     <t>Hong Kong residents aged from 15 days to 80 years old</t>
@@ -3772,19 +3744,6 @@
   </si>
   <si>
     <t>If I use Treatment Sure as CoreChoice policy holder, will Prudential pay for my overseas treatment costs?</t>
-  </si>
-  <si>
-    <t>If you are a CoreChoice policyholder and use the Treatment Sure service, Prudential does not directly pay for your overseas treatment costs. Here’s how it works specifically in the context of CoreChoice and Treatment Sure:
-Treatment Sure Services:
-Treatment Sure provides access to:
-Global Expert Medical Opinion.
-Overseas Medical Concierge services.
-These services assist in arranging your overseas treatment, but Prudential does not cover the travel, accommodation, or related costs involved.
-Claiming Treatment Costs:
-Only the actual treatment expenses are claimable under the benefit limits specified by your CoreChoice plan. Any such claims must adhere to the plan's terms and pre-authorization requirements.
-Source Quote:
-“The amount you can claim for treatment expenses is subject to the benefit limit of your plan… You will need to get our pre-authorisation before your treatment.”
-(Source: PRUHealth CoreChoice Product Documentation)</t>
   </si>
   <si>
     <t>If I become mentally incapacitated, does SmartAppoint Service guarantee my family can access my claims under CoreChoice?</t>
@@ -4159,12 +4118,151 @@
   <si>
     <t>corpus match</t>
   </si>
+  <si>
+    <t>Treatment Sure is a one-stop medical advisory service provided by Prudential in collaboration with its partner, Teladoc Health. This service includes:
+Global Second Medical Opinions: Offers independent medical opinions from an extensive network of over 50,000 global medical experts covering more than 450 specialties and sub-specialties. This helps you verify diagnoses and explore the most suitable treatments for your condition.
+Medical Concierge for Overseas Treatment: If you need treatment abroad, the service provides a dedicated physician case manager to guide you throughout your medical journey. This includes identifying suitable specialists around the world, arranging appointments, translation services, and even follow-ups post-treatment.
+Comprehensive Support: A dedicated physician case manager is assigned to support you at every step, answering your questions and ensuring personalized care.
+The service has benefited over 35 million customers across 130 countries, assuring peace of mind by helping in making informed health decisions.
+How Does It Work?
+Step 1: A physician case manager is assigned to you.
+Step 2: The manager gathers details about your medical condition.
+Step 3: Suitable global experts are identified and consulted.
+Step 4: You receive a personalized second medical opinion report in your language.
+Step 5: If you opt for overseas treatment, the manager organizes specialist options, appointments, and logistics.
+Step 6: Post-treatment, the manager follows up on your recovery.
+Contact Details
+For activation or queries:
+Hong Kong SAR: (852) 8229 2880
+Mainland China: (86) 400 920 6012</t>
+  </si>
+  <si>
+    <t>If you are a CoreChoice policyholder and use the Treatment Sure service, Prudential does not directly pay for your overseas treatment costs. Here’s how it works specifically in the context of CoreChoice and Treatment Sure:
+Treatment Sure Services:
+Treatment Sure provides access to:
+Global Expert Medical Opinion.
+Overseas Medical Concierge services.
+These services assist in arranging your overseas treatment, but Prudential does not cover the travel, accommodation, or related costs involved.
+Claiming Treatment Costs:
+Only the actual treatment expenses are claimable under the benefit limits specified by your CoreChoice plan. Any such claims must adhere to the plan's terms and pre-authorization requirements.</t>
+  </si>
+  <si>
+    <t>gs://guide-care-poc/policy/dbso-flyer.pdf</t>
+  </si>
+  <si>
+    <t>gs://guide-care-poc/policy/premierflex-medical-plan-product-brochure_hk.pdf</t>
+  </si>
+  <si>
+    <t>Medical Protection
+PremierFlex Medical Plan
+Lifetime freedom for medical treatment with coverage 
+in Macau, China and worldwide, all from one plan
+Macau Edition
+Health
+Care2
+The PremierFlex Medical Plan provides lifetime renewal, fully covering 
+your eligible medical costs for major benefit items and comprehensively 
+supporting you through prevention, diagnosis and treatment to recovery. 
+You can select your coverage area (Greater China, worldwide (except the USA) or 
+worldwide) as well as your deductible. Stay in a standard single room
+(including a qualified room in VIP units and international units) at hospitals in 
+mainland China, or a semi-private / private room in Hong Kong, Macau and 
+other regions, with premium quality medical service. Based on your needs, you can 
+also opt for a designated supplementary outpatient benefit â€“ â€œOutpatient Care 
+Benefitâ€ â€“ for outpatient treatment anytime in mainland China, Hong Kong and 
+Macau, giving you extra peace of mind.
+Through the HealthCare+ e-platform, we support you with a series of 
+thoughtful and dedicated value-added services â€“ including medical 
+green channels, direct billing for medical expenses, second medical 
+opinion and global drug search. This ensures you can obtain support for both 
+minor ailments and major illnesses.
+PremierFlex Medical Plan giving you access to top-notch medical service for 
+life, truly achieving healthcare freedom.
+PremierFlex Medical Plan3 4
+Plan highlights
+The PremierFlex Medical Plan offers 4 plans, with different coverage areas, giving you comprehensive protection â€“ from prevention, diagnosis, treatment to recovery wherever you are. Even if your medical history changes or there is a claim on the plan, 
+we will renew your plan every year throughout your lifetime, providing you with lifelong protection. The medical coverage includes:
+ You can also access Rare-in-Hong Kong market one-stop dedicated value-added services through the HealthCare+, 
+giving you help for both minor ailments and major illnesses. These include:
+â—†Full cover for eligible medical costs of prescribed diagnostic 
+imaging tests
+â—†Full cover for eligible medical costs of outpatient consultation 
+before hospitalisation or day case procedure
+â—†ã€Optional supplementary benefitã€‘Outpatient benefit â€“ 
+Outpatient Care Benefit applies to any hospital or clinic
+in mainland China, Hong Kong and Macau, covers outpatient 
+consultations, laboratory tests and diagnostic imaging as well 
+as Rare-in-Hong Kong market telemedicine service and 
+medication delivery (in mainland China)
+â—†Full cover for eligible medical costs for follow-up outpatient 
+consultations after a hospital stay or day case procedure. 
+We will extend the coverage period by 4 times to 365 days
+for complex or major surgery
+â—†Cover for eligible medical costs for rehabilitation care, including 
+traditional Chinese medicine (including acupuncture) during 
+rehabilitation, and daily post-surgery home nursing, etc.
+â—† Rare-in-Hong Kong and 
+the mainland China market Extra rehabilitation care for 
+covered cancer, heart attack and stroke
+â—†Health Consultant
+â—†Medical Concierge and Escort
+â—†Second Medical Opinion
+â—†Worldwide Emergency Assistance
+â—†Medical Green Channel in 
+mainland China 
+â—†Medical Expenses Direct Billing
+â—†SmartAppoint (advanced appointment 
+of designated person for claims)
+â—†Personalised Rehabilitation 
+Assessment
+â—†Specialist Tailored-made 
+Rehabilitation Guidance Plan
+â—†Dedicated Critical Illness Case Manager
+â—†Critical Illness Counselling
+â—† Rare-in-Hong Kong and 
+the mainland China market
+Greater Bay Area Cross-border Cancer 
+Treatment Medical Expenses Direct Billing
+â—† Rare-in-Hong Kong market
+Global Drug Search
+â—† Rare-in-Hong Kong market
+Drug Discount
+â—†Healthcare Service Discount
+Personalised 
+Treatment Assistance Hassle-free Admission, 
+Direct Billing and Claims
+Medication and 
+Healthcare
+Professional Critical Illness
+Management
+Tailored Rehabilitation 
+Care
+Prevention Diagnosis Treatment
+â—†We cover over 14,000â€  2-Grade or above hospitals in mainland China. 
+Rare-in-Hong Kong market No matter which plan you choose, 
+we fully cover your major eligible inpatient and surgical costs when 
+you stay in a standard single room (covers a qualified room in 
+VIP units and international units) in public hospitals in mainland 
+China.</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>What is the annual benefit limit under pruhealth CoreChoice?</t>
+  </si>
+  <si>
+    <t>What's Treatment Sure? I am a policy holder for PRUmyhealth prestige medical plan.</t>
+  </si>
+  <si>
+    <t>Who is eligible to apply for pruhealth CoreChoice? I am a policy holder</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4176,13 +4274,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FFFAFAFA"/>
-      <name val="Source Sans Pro"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -4311,12 +4402,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8793,8 +8886,8 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8803,7 +8896,7 @@
     <col min="2" max="2" width="32" style="3" customWidth="1"/>
     <col min="3" max="3" width="45.85546875" style="3" customWidth="1"/>
     <col min="4" max="4" width="51.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="5" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8816,14 +8909,14 @@
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>581</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>582</v>
       </c>
-      <c r="F1" s="18" t="s">
-        <v>647</v>
+      <c r="F1" s="17" t="s">
+        <v>642</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
@@ -8834,56 +8927,56 @@
         <v>584</v>
       </c>
       <c r="C2" s="16" t="s">
+        <v>643</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>585</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="16" t="s">
         <v>586</v>
       </c>
-      <c r="E2" s="16" t="s">
-        <v>587</v>
-      </c>
-      <c r="F2" t="s">
-        <v>645</v>
+      <c r="F2" s="18" t="s">
+        <v>640</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>588</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="C3" s="16" t="s">
         <v>589</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="D3" s="16" t="s">
         <v>590</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="16" t="s">
         <v>591</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>592</v>
-      </c>
-      <c r="F3" t="s">
-        <v>646</v>
+      <c r="F3" s="18" t="s">
+        <v>641</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>650</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>593</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="D4" s="16" t="s">
         <v>594</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="E4" s="16" t="s">
         <v>595</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>596</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>597</v>
-      </c>
-      <c r="F4" t="s">
-        <v>646</v>
+      <c r="F4" s="18" t="s">
+        <v>641</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="250.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8894,16 +8987,16 @@
         <v>402</v>
       </c>
       <c r="C5" s="16" t="s">
+        <v>596</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>597</v>
+      </c>
+      <c r="E5" s="16" t="s">
         <v>598</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>599</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>600</v>
-      </c>
-      <c r="F5" t="s">
-        <v>646</v>
+      <c r="F5" s="18" t="s">
+        <v>641</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="262.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8911,19 +9004,19 @@
         <v>583</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>601</v>
+        <v>649</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>602</v>
-      </c>
-      <c r="D6" s="3" t="s">
         <v>599</v>
       </c>
+      <c r="D6" s="16" t="s">
+        <v>597</v>
+      </c>
       <c r="E6" s="16" t="s">
-        <v>600</v>
-      </c>
-      <c r="F6" t="s">
-        <v>646</v>
+        <v>598</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>641</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
@@ -8931,139 +9024,139 @@
         <v>583</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>603</v>
+        <v>651</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>604</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>599</v>
+        <v>600</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>597</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>600</v>
-      </c>
-      <c r="F7" t="s">
-        <v>646</v>
+        <v>598</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>641</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>606</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>607</v>
+        <v>602</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>603</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>600</v>
-      </c>
-      <c r="F8" t="s">
-        <v>646</v>
+        <v>598</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>641</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>609</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>599</v>
+        <v>605</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>597</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>600</v>
-      </c>
-      <c r="F9" t="s">
-        <v>646</v>
+        <v>598</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>641</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>611</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>612</v>
+        <v>607</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>608</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>613</v>
-      </c>
-      <c r="F10" t="s">
-        <v>645</v>
+        <v>609</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>640</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>615</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>607</v>
+        <v>644</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>603</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>600</v>
-      </c>
-      <c r="F11" t="s">
-        <v>646</v>
+        <v>598</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>641</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B12" s="16" t="s">
+        <v>611</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>612</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>613</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>614</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="174.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>615</v>
+      </c>
+      <c r="C13" s="16" t="s">
         <v>616</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="D13" s="16" t="s">
         <v>617</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E13" s="16" t="s">
         <v>618</v>
       </c>
-      <c r="E12" s="16" t="s">
-        <v>619</v>
-      </c>
-      <c r="F12" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>593</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>620</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>621</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>622</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>623</v>
-      </c>
-      <c r="F13" t="s">
-        <v>645</v>
+      <c r="F13" s="18" t="s">
+        <v>640</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
@@ -9071,135 +9164,159 @@
         <v>583</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>625</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>626</v>
+        <v>620</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>621</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>627</v>
-      </c>
-      <c r="F14" t="s">
-        <v>645</v>
+        <v>622</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>640</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="300" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>629</v>
-      </c>
-      <c r="F15" t="s">
+        <v>624</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>648</v>
+      </c>
+      <c r="E15" s="16" t="s">
         <v>645</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>641</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="255" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B16" s="16" t="s">
+        <v>625</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>626</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>648</v>
+      </c>
+      <c r="E16" s="16" t="s">
         <v>630</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="F16" s="18" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>587</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>627</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>628</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>629</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>630</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="B18" s="16" t="s">
         <v>631</v>
       </c>
-      <c r="F16" t="s">
+      <c r="C18" s="16" t="s">
+        <v>632</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>647</v>
+      </c>
+      <c r="E18" s="16" t="s">
         <v>646</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>588</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>632</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>633</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>634</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>635</v>
-      </c>
-      <c r="F17" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
-        <v>593</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>636</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>637</v>
-      </c>
-      <c r="F18" t="s">
-        <v>646</v>
+      <c r="F18" s="18" t="s">
+        <v>641</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>593</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>638</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>639</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>626</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>627</v>
-      </c>
-      <c r="F19" t="s">
-        <v>645</v>
+        <v>592</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>633</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>634</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>622</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>640</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>593</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>640</v>
-      </c>
-      <c r="C20" s="3" t="s">
+        <v>592</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>635</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>636</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>648</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>591</v>
+      </c>
+      <c r="F20" s="18" t="s">
         <v>641</v>
       </c>
-      <c r="F20" t="s">
-        <v>646</v>
-      </c>
     </row>
     <row r="21" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
-        <v>588</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>642</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>644</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>597</v>
-      </c>
-      <c r="F21" t="s">
-        <v>646</v>
+      <c r="A21" s="19" t="s">
+        <v>587</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>637</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>638</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>639</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>595</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>641</v>
       </c>
     </row>
   </sheetData>

</xml_diff>